<commit_message>
Project 2: Begin and outline
</commit_message>
<xml_diff>
--- a/Schedule/Quant II Recitation - Spring 2015.xlsx
+++ b/Schedule/Quant II Recitation - Spring 2015.xlsx
@@ -178,9 +178,6 @@
     <t>LPM</t>
   </si>
   <si>
-    <t>specification/functional form</t>
-  </si>
-  <si>
     <t>Graphing Subgroups</t>
   </si>
   <si>
@@ -278,9 +275,6 @@
   </si>
   <si>
     <t>non-independence</t>
-  </si>
-  <si>
-    <t>measurement</t>
   </si>
   <si>
     <t>regression topics</t>
@@ -384,6 +378,14 @@
   </si>
   <si>
     <t xml:space="preserve"> predicted values</t>
+  </si>
+  <si>
+    <t>specification/functional form
+midterm</t>
+  </si>
+  <si>
+    <t>measurement
+midterm</t>
   </si>
 </sst>
 </file>
@@ -439,7 +441,7 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -461,6 +463,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,7 +503,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -575,6 +583,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1142,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="48.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1185,7 @@
         <v>1</v>
       </c>
       <c r="H1" s="24" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I1" s="25"/>
       <c r="J1" s="25"/>
@@ -1244,7 +1255,7 @@
     </row>
     <row r="4" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
@@ -1292,7 +1303,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>27</v>
@@ -1329,7 +1340,7 @@
         <v>33</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="11" t="s">
@@ -1358,7 +1369,7 @@
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="28" t="s">
         <v>40</v>
       </c>
       <c r="I7" s="11" t="s">
@@ -1374,7 +1385,7 @@
     </row>
     <row r="8" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B8" s="13">
         <v>4</v>
@@ -1397,8 +1408,8 @@
       <c r="H8" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="11" t="s">
-        <v>48</v>
+      <c r="I8" s="28" t="s">
+        <v>104</v>
       </c>
       <c r="J8" s="11" t="s">
         <v>36</v>
@@ -1419,29 +1430,29 @@
         <v>42065</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="H9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="I9" s="11" t="s">
+      <c r="J9" s="28" t="s">
         <v>53</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="K9" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="L9" s="11" t="s">
-        <v>54</v>
+      <c r="L9" s="28" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1449,13 +1460,13 @@
         <v>42072</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>47</v>
@@ -1466,7 +1477,7 @@
     </row>
     <row r="11" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B11" s="13">
         <v>6</v>
@@ -1475,29 +1486,29 @@
         <v>42079</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="J11" s="11" t="s">
         <v>60</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>61</v>
       </c>
       <c r="K11" s="11" t="s">
         <v>47</v>
       </c>
       <c r="L11" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1509,84 +1520,84 @@
         <v>42086</v>
       </c>
       <c r="D12" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="F12" s="15" t="s">
         <v>63</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="F12" s="15" t="s">
-        <v>64</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I12" s="11" t="s">
         <v>65</v>
-      </c>
-      <c r="I12" s="11" t="s">
-        <v>66</v>
       </c>
       <c r="J12" s="11" t="s">
         <v>47</v>
       </c>
       <c r="K12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="L12" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="L12" s="11" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C13" s="21" t="s">
+        <v>68</v>
+      </c>
+      <c r="D13" s="17" t="s">
         <v>69</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>70</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="J13" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="11" t="s">
         <v>72</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="L13" s="11" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
       <c r="H14" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
+      </c>
+      <c r="I14" s="28" t="s">
+        <v>105</v>
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L14" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B15" s="16">
         <v>8</v>
@@ -1595,29 +1606,29 @@
         <v>42107</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E15" s="15" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="11" t="s">
+      <c r="K15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="L15" s="11" t="s">
         <v>82</v>
-      </c>
-      <c r="J15" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="L15" s="11" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1629,29 +1640,29 @@
         <v>42114</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G16" s="15"/>
       <c r="H16" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I16" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K16" s="11" t="s">
         <v>18</v>
       </c>
       <c r="L16" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:12" ht="48.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -1665,13 +1676,13 @@
       <c r="G17" s="16"/>
       <c r="H17" s="11"/>
       <c r="I17" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="K17" s="11" t="s">
         <v>90</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>92</v>
       </c>
       <c r="L17" s="11"/>
     </row>

</xml_diff>